<commit_message>
plots working better now
</commit_message>
<xml_diff>
--- a/data/Demo BoD.xlsx
+++ b/data/Demo BoD.xlsx
@@ -1075,27 +1075,27 @@
     <t xml:space="preserve">B.1.7.1</t>
   </si>
   <si>
+    <t xml:space="preserve">Liver cancer due to NASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B.1.7.2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liver cancer due to alcohol use</t>
   </si>
   <si>
-    <t xml:space="preserve">B.1.7.2</t>
+    <t xml:space="preserve">B.1.7.4</t>
   </si>
   <si>
     <t xml:space="preserve">Liver cancer due to hepatitis B</t>
   </si>
   <si>
-    <t xml:space="preserve">B.1.7.4</t>
+    <t xml:space="preserve">B.1.7.3</t>
   </si>
   <si>
     <t xml:space="preserve">Liver cancer due to hepatitis C</t>
   </si>
   <si>
-    <t xml:space="preserve">B.1.7.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liver cancer due to NASH</t>
-  </si>
-  <si>
     <t xml:space="preserve">B.1.7.5</t>
   </si>
   <si>
@@ -1348,13 +1348,13 @@
     <t xml:space="preserve">Neurological disorders</t>
   </si>
   <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-communicable diseases</t>
+  </si>
+  <si>
     <t xml:space="preserve">B.1.26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-communicable diseases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
   </si>
   <si>
     <t xml:space="preserve">Non-Hodgkin lymphoma</t>
@@ -2331,8 +2331,8 @@
   </sheetPr>
   <dimension ref="A1:F361"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A147" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C165" activeCellId="0" sqref="C165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5817,13 +5817,13 @@
         <v>351</v>
       </c>
       <c r="D174" s="1" t="n">
-        <v>1547.19142345038</v>
+        <v>1471.91919337854</v>
       </c>
       <c r="E174" s="1" t="n">
-        <v>59.1158687613433</v>
+        <v>56.1139288126655</v>
       </c>
       <c r="F174" s="1" t="n">
-        <v>64.2830811154</v>
+        <v>59.4720717303</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5837,13 +5837,13 @@
         <v>353</v>
       </c>
       <c r="D175" s="1" t="n">
-        <v>7795.36390018066</v>
+        <v>1547.19142345038</v>
       </c>
       <c r="E175" s="1" t="n">
-        <v>216.567251231455</v>
+        <v>59.1158687613433</v>
       </c>
       <c r="F175" s="1" t="n">
-        <v>289.114844363</v>
+        <v>64.2830811154</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5857,13 +5857,13 @@
         <v>355</v>
       </c>
       <c r="D176" s="1" t="n">
-        <v>5280.67045704024</v>
+        <v>7795.36390018066</v>
       </c>
       <c r="E176" s="1" t="n">
-        <v>212.286893227244</v>
+        <v>216.567251231455</v>
       </c>
       <c r="F176" s="1" t="n">
-        <v>220.763337792</v>
+        <v>289.114844363</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5877,13 +5877,13 @@
         <v>357</v>
       </c>
       <c r="D177" s="1" t="n">
-        <v>1471.91919337854</v>
+        <v>5280.67045704024</v>
       </c>
       <c r="E177" s="1" t="n">
-        <v>56.1139288126655</v>
+        <v>212.286893227244</v>
       </c>
       <c r="F177" s="1" t="n">
-        <v>59.4720717303</v>
+        <v>220.763337792</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6728,7 +6728,7 @@
     </row>
     <row r="220" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B220" s="0" t="s">
         <v>442</v>
@@ -6748,7 +6748,7 @@
     </row>
     <row r="221" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B221" s="0" t="s">
         <v>444</v>

</xml_diff>